<commit_message>
added tooltips, and women to ship menu
</commit_message>
<xml_diff>
--- a/datasets/ShippedCharacters.xlsx
+++ b/datasets/ShippedCharacters.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emily\Documents\Cornell\INFO4310\fanfiction\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6ABBB97-602A-4B08-92DA-B94A92A0E4C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5676A4C-544D-4407-847B-DD31A9159221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="15466" xr2:uid="{4B3C2D8F-8A3B-480C-9494-7DF2955BE3AB}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="characters" sheetId="1" r:id="rId1"/>
+    <sheet name="Media" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="100">
   <si>
     <t>Character</t>
   </si>
@@ -203,9 +204,6 @@
     <t>Alec Lightwood</t>
   </si>
   <si>
-    <t xml:space="preserve">Supernatural </t>
-  </si>
-  <si>
     <t>Media</t>
   </si>
   <si>
@@ -234,6 +232,111 @@
   </si>
   <si>
     <t>Animated TV Series</t>
+  </si>
+  <si>
+    <t>Hermione Granger</t>
+  </si>
+  <si>
+    <t>Rey</t>
+  </si>
+  <si>
+    <t>Star Wars</t>
+  </si>
+  <si>
+    <t>Kylo Ren</t>
+  </si>
+  <si>
+    <t>Ron Weasley</t>
+  </si>
+  <si>
+    <t>Pepper Potts</t>
+  </si>
+  <si>
+    <t>Kara Danvers</t>
+  </si>
+  <si>
+    <t>Supergirl</t>
+  </si>
+  <si>
+    <t>Lena Luthor</t>
+  </si>
+  <si>
+    <t>Emma Swan</t>
+  </si>
+  <si>
+    <t>Once Upon A Time</t>
+  </si>
+  <si>
+    <t>Regina Mills</t>
+  </si>
+  <si>
+    <t>Amity Blight</t>
+  </si>
+  <si>
+    <t>The Owl House</t>
+  </si>
+  <si>
+    <t>Luz Noceda</t>
+  </si>
+  <si>
+    <t>The 100</t>
+  </si>
+  <si>
+    <t>Clarke Griffin</t>
+  </si>
+  <si>
+    <t>Lexa</t>
+  </si>
+  <si>
+    <t>Drama</t>
+  </si>
+  <si>
+    <t>Adora</t>
+  </si>
+  <si>
+    <t>She-Ra and the Princesses of Power</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Catra</t>
+  </si>
+  <si>
+    <t>Robin Buckley</t>
+  </si>
+  <si>
+    <t>Stranger Things</t>
+  </si>
+  <si>
+    <t>Nancy Wheeler</t>
+  </si>
+  <si>
+    <t>Yang Xiao Long</t>
+  </si>
+  <si>
+    <t>RWBY</t>
+  </si>
+  <si>
+    <t>Blake Belladonna</t>
+  </si>
+  <si>
+    <t>Korra</t>
+  </si>
+  <si>
+    <t>The Legend of Korra</t>
+  </si>
+  <si>
+    <t>Asami Sato</t>
+  </si>
+  <si>
+    <t>Caitlyn Kiramman</t>
+  </si>
+  <si>
+    <t>Arcane</t>
+  </si>
+  <si>
+    <t>Vi (Violet)</t>
   </si>
 </sst>
 </file>
@@ -614,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3606BCCE-A98D-4571-A7A4-98E1447D4C81}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:C59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -627,7 +730,7 @@
     <col min="3" max="3" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,27 +738,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -663,13 +760,10 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -677,13 +771,10 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -691,41 +782,32 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>13</v>
       </c>
@@ -733,13 +815,10 @@
         <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -747,13 +826,10 @@
         <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -761,13 +837,10 @@
         <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -775,13 +848,10 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -789,13 +859,10 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -803,13 +870,10 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -817,13 +881,10 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -831,13 +892,10 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -845,13 +903,10 @@
         <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -859,13 +914,10 @@
         <v>26</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A18" t="s">
         <v>28</v>
       </c>
@@ -873,41 +925,32 @@
         <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.5">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="B19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A21" t="s">
         <v>32</v>
       </c>
@@ -915,13 +958,10 @@
         <v>34</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A22" t="s">
         <v>33</v>
       </c>
@@ -929,13 +969,10 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A23" t="s">
         <v>35</v>
       </c>
@@ -943,13 +980,10 @@
         <v>36</v>
       </c>
       <c r="C23" t="s">
-        <v>37</v>
-      </c>
-      <c r="D23" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -957,13 +991,10 @@
         <v>36</v>
       </c>
       <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.5">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -971,13 +1002,10 @@
         <v>40</v>
       </c>
       <c r="C25" t="s">
-        <v>21</v>
-      </c>
-      <c r="D25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -985,13 +1013,10 @@
         <v>40</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A27" t="s">
         <v>42</v>
       </c>
@@ -999,13 +1024,10 @@
         <v>42</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
-      </c>
-      <c r="D27" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A28" t="s">
         <v>43</v>
       </c>
@@ -1013,13 +1035,10 @@
         <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>5</v>
-      </c>
-      <c r="D28" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1027,13 +1046,10 @@
         <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1041,13 +1057,10 @@
         <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
-      </c>
-      <c r="D30" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.5">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1055,13 +1068,10 @@
         <v>48</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A32" t="s">
         <v>49</v>
       </c>
@@ -1069,13 +1079,10 @@
         <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>5</v>
-      </c>
-      <c r="D32" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A33" t="s">
         <v>50</v>
       </c>
@@ -1083,13 +1090,10 @@
         <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>5</v>
-      </c>
-      <c r="D33" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.5">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A34" t="s">
         <v>51</v>
       </c>
@@ -1097,13 +1101,10 @@
         <v>26</v>
       </c>
       <c r="C34" t="s">
-        <v>21</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.5">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A35" t="s">
         <v>52</v>
       </c>
@@ -1111,13 +1112,10 @@
         <v>53</v>
       </c>
       <c r="C35" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.5">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A36" t="s">
         <v>54</v>
       </c>
@@ -1125,14 +1123,878 @@
         <v>53</v>
       </c>
       <c r="C36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" t="s">
-        <v>57</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" t="s">
+        <v>8</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="B39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
+        <v>20</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>71</v>
+      </c>
+      <c r="B42" t="s">
+        <v>72</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
+        <v>74</v>
+      </c>
+      <c r="B44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A45" t="s">
+        <v>76</v>
+      </c>
+      <c r="B45" t="s">
+        <v>75</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
+        <v>77</v>
+      </c>
+      <c r="B46" t="s">
+        <v>78</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" t="s">
+        <v>78</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
+        <v>81</v>
+      </c>
+      <c r="B48" t="s">
+        <v>80</v>
+      </c>
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A49" t="s">
+        <v>82</v>
+      </c>
+      <c r="B49" t="s">
+        <v>80</v>
+      </c>
+      <c r="C49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A50" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A51" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" t="s">
+        <v>85</v>
+      </c>
+      <c r="C51" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A52" t="s">
+        <v>88</v>
+      </c>
+      <c r="B52" t="s">
+        <v>89</v>
+      </c>
+      <c r="C52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A54" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" t="s">
+        <v>92</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A55" t="s">
+        <v>93</v>
+      </c>
+      <c r="B55" t="s">
+        <v>92</v>
+      </c>
+      <c r="C55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A56" t="s">
+        <v>94</v>
+      </c>
+      <c r="B56" t="s">
+        <v>95</v>
+      </c>
+      <c r="C56" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
+        <v>96</v>
+      </c>
+      <c r="B57" t="s">
+        <v>95</v>
+      </c>
+      <c r="C57" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
+        <v>97</v>
+      </c>
+      <c r="B58" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A59" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" t="s">
+        <v>98</v>
+      </c>
+      <c r="C59" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C55A625-B8A0-4C94-B781-BDC0CD8D3B65}">
+  <dimension ref="A1:C59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="28.8203125" customWidth="1"/>
+    <col min="2" max="2" width="25.1171875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
+        <v>62</v>
+      </c>
+      <c r="B19" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A22" t="s">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="B26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A29" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A32" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A34" t="s">
+        <v>26</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A35" t="s">
+        <v>53</v>
+      </c>
+      <c r="B35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A36" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A38" t="s">
+        <v>67</v>
+      </c>
+      <c r="B38" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="B39" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" t="s">
+        <v>21</v>
+      </c>
+      <c r="C41" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
+        <v>21</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A43" t="s">
+        <v>72</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A46" t="s">
+        <v>78</v>
+      </c>
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A47" t="s">
+        <v>78</v>
+      </c>
+      <c r="B47" t="s">
+        <v>5</v>
+      </c>
+      <c r="C47" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A48" t="s">
+        <v>80</v>
+      </c>
+      <c r="B48" t="s">
+        <v>83</v>
+      </c>
+      <c r="C48" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A49" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" t="s">
+        <v>83</v>
+      </c>
+      <c r="C49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A50" t="s">
+        <v>85</v>
+      </c>
+      <c r="B50" t="s">
+        <v>86</v>
+      </c>
+      <c r="C50" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A51" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A52" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A53" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A54" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A55" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A56" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A57" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A58" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A59" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>